<commit_message>
demo forms, tasks and targets
</commit_message>
<xml_diff>
--- a/forms/app/ebs_assessment_training.xlsx
+++ b/forms/app/ebs_assessment_training.xlsx
@@ -22,7 +22,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="288" uniqueCount="188">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="321" uniqueCount="213">
   <si>
     <t xml:space="preserve">type</t>
   </si>
@@ -42,6 +42,9 @@
     <t xml:space="preserve">appearance</t>
   </si>
   <si>
+    <t xml:space="preserve">body::intent</t>
+  </si>
+  <si>
     <t xml:space="preserve">constraint</t>
   </si>
   <si>
@@ -117,6 +120,12 @@
     <t xml:space="preserve">_id</t>
   </si>
   <si>
+    <t xml:space="preserve">phone</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Phone</t>
+  </si>
+  <si>
     <t xml:space="preserve">calculate</t>
   </si>
   <si>
@@ -129,10 +138,16 @@
     <t xml:space="preserve">../inputs/contact/_id</t>
   </si>
   <si>
+    <t xml:space="preserve">patient_phone</t>
+  </si>
+  <si>
+    <t xml:space="preserve">../inputs/contact/phone</t>
+  </si>
+  <si>
     <t xml:space="preserve">ebs_intro</t>
   </si>
   <si>
-    <t xml:space="preserve">Event-Based Surveillance</t>
+    <t xml:space="preserve">Covid-19 Education</t>
   </si>
   <si>
     <t xml:space="preserve">note</t>
@@ -144,12 +159,57 @@
     <t xml:space="preserve">**Thank you for serving your community with event-based surveillance**</t>
   </si>
   <si>
+    <t xml:space="preserve">send_message</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Click to send sms note</t>
+  </si>
+  <si>
+    <t xml:space="preserve">ex:android.intent.action.SENDTO(uri_data='smsto:12345678', sms_body=${thanking_note})</t>
+  </si>
+  <si>
     <t xml:space="preserve">covid_introduction</t>
   </si>
   <si>
     <t xml:space="preserve">To avoid infection of yourself and others with COVID-19, it is important to practice the following hygiene measures:</t>
   </si>
   <si>
+    <t xml:space="preserve">learning_objectives</t>
+  </si>
+  <si>
+    <t xml:space="preserve">**Learning Objectives**</t>
+  </si>
+  <si>
+    <t xml:space="preserve">hand_hygiene</t>
+  </si>
+  <si>
+    <t xml:space="preserve">1. Know effective hand hygiene practices</t>
+  </si>
+  <si>
+    <t xml:space="preserve">infected_secretions</t>
+  </si>
+  <si>
+    <t xml:space="preserve">2. Know the correct way to handle infected secretions from the nose, eyes and mouth</t>
+  </si>
+  <si>
+    <t xml:space="preserve">household_hygiene</t>
+  </si>
+  <si>
+    <t xml:space="preserve">3. Know good household hygiene practices</t>
+  </si>
+  <si>
+    <t xml:space="preserve">distancing</t>
+  </si>
+  <si>
+    <t xml:space="preserve">4. Know when to self-distance and self-quarantine</t>
+  </si>
+  <si>
+    <t xml:space="preserve">reporting_cases</t>
+  </si>
+  <si>
+    <t xml:space="preserve">5. Know when to report a patient with suspected infection to the local health authorities</t>
+  </si>
+  <si>
     <t xml:space="preserve">isolate</t>
   </si>
   <si>
@@ -378,25 +438,49 @@
     <t xml:space="preserve">result</t>
   </si>
   <si>
-    <t xml:space="preserve">Results</t>
-  </si>
-  <si>
-    <t xml:space="preserve">h1 blue</t>
+    <t xml:space="preserve">Thank you</t>
+  </si>
+  <si>
+    <t xml:space="preserve">h1 green</t>
   </si>
   <si>
     <t xml:space="preserve">success_1</t>
   </si>
   <si>
-    <t xml:space="preserve">Great job! You have answered all the questions correctly. Your EBS training is complete!</t>
+    <t xml:space="preserve">You have answered all the questions correctly! You may review this content on your profile page.</t>
   </si>
   <si>
     <t xml:space="preserve">${assessment_passed} = ‘yes’</t>
   </si>
   <si>
-    <t xml:space="preserve">success_2</t>
-  </si>
-  <si>
-    <t xml:space="preserve">You may now start reporting on households using EBS.</t>
+    <t xml:space="preserve">select_one confidence_level</t>
+  </si>
+  <si>
+    <t xml:space="preserve">success_confidence</t>
+  </si>
+  <si>
+    <t xml:space="preserve">How confident do you feel in your mastery of this content?</t>
+  </si>
+  <si>
+    <t xml:space="preserve">select_one yes_no</t>
+  </si>
+  <si>
+    <t xml:space="preserve">effective_performance</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Will you be able to effectively perform the task?</t>
+  </si>
+  <si>
+    <t xml:space="preserve">text</t>
+  </si>
+  <si>
+    <t xml:space="preserve">feedback</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Do you have any other questions or feedback on this topic? (Optional)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Your supervisor will follow up</t>
   </si>
   <si>
     <t xml:space="preserve">fail_1</t>
@@ -414,61 +498,19 @@
     <t xml:space="preserve">We’ll generate another task for you to go through the workflow again.</t>
   </si>
   <si>
-    <t xml:space="preserve">fail_3</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Please review the following and resubmit:</t>
-  </si>
-  <si>
-    <t xml:space="preserve">hand_wash_sug</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Handwashing (and its ability to prevent covid)</t>
-  </si>
-  <si>
-    <t xml:space="preserve">${hand_washing_q} != ‘both_soap_and_water_or_hand_saniter’</t>
-  </si>
-  <si>
-    <t xml:space="preserve">li</t>
-  </si>
-  <si>
-    <t xml:space="preserve">hand_wash_duration_sug</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Handwashing (and required duration for effectiveness)</t>
-  </si>
-  <si>
-    <t xml:space="preserve">${hand_wash_duration_q} != ‘at_least_20_seconds’</t>
-  </si>
-  <si>
-    <t xml:space="preserve">sneeze_cough_sug</t>
-  </si>
-  <si>
-    <t xml:space="preserve">${sneezing_coughing_q} != ‘cough_into_your_elbow_or_tissue’ </t>
-  </si>
-  <si>
-    <t xml:space="preserve">household_sug</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Houshold</t>
-  </si>
-  <si>
-    <t xml:space="preserve">${household_q} != ‘a_disinfectant’</t>
-  </si>
-  <si>
-    <t xml:space="preserve">social_distance_sug</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Social Distancing</t>
-  </si>
-  <si>
-    <t xml:space="preserve">${social_distancing_q} != ‘at_least_2_meters’</t>
-  </si>
-  <si>
-    <t xml:space="preserve">fail_4</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Educating ourselves and the community is the best way to stop covid.</t>
+    <t xml:space="preserve">Fail_3</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Thank you for your persistence, educating ourselves and our communities is the best way to stop covid.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">fail_assistance</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Do you need assistance with this topic?</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Optional</t>
   </si>
   <si>
     <t xml:space="preserve">list_name</t>
@@ -558,6 +600,39 @@
     <t xml:space="preserve">At least 2 meters</t>
   </si>
   <si>
+    <t xml:space="preserve">confidence_level</t>
+  </si>
+  <si>
+    <t xml:space="preserve">extreme</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Extremely confident</t>
+  </si>
+  <si>
+    <t xml:space="preserve">very</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Very confident</t>
+  </si>
+  <si>
+    <t xml:space="preserve">somewhat</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Somewhat confident</t>
+  </si>
+  <si>
+    <t xml:space="preserve">a_little</t>
+  </si>
+  <si>
+    <t xml:space="preserve">A little confident</t>
+  </si>
+  <si>
+    <t xml:space="preserve">no_confidence</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Not confident at all</t>
+  </si>
+  <si>
     <t xml:space="preserve">form_title</t>
   </si>
   <si>
@@ -576,7 +651,7 @@
     <t xml:space="preserve">instance_name</t>
   </si>
   <si>
-    <t xml:space="preserve">EBS Training</t>
+    <t xml:space="preserve">Training</t>
   </si>
   <si>
     <t xml:space="preserve">ebs_assessment_training</t>
@@ -727,7 +802,7 @@
     <xf numFmtId="42" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
   </cellStyleXfs>
-  <cellXfs count="12">
+  <cellXfs count="13">
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
@@ -757,6 +832,10 @@
       <protection locked="true" hidden="false"/>
     </xf>
     <xf numFmtId="164" fontId="0" fillId="4" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -946,30 +1025,30 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:BA69"/>
+  <dimension ref="A1:BB75"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="80" zoomScaleNormal="80" zoomScalePageLayoutView="100" workbookViewId="0">
-      <pane xSplit="1" ySplit="1" topLeftCell="B12" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="1" ySplit="1" topLeftCell="B8" activePane="bottomRight" state="frozen"/>
       <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
       <selection pane="topRight" activeCell="B1" activeCellId="0" sqref="B1"/>
-      <selection pane="bottomLeft" activeCell="A12" activeCellId="0" sqref="A12"/>
-      <selection pane="bottomRight" activeCell="C15" activeCellId="0" sqref="C15"/>
+      <selection pane="bottomLeft" activeCell="A8" activeCellId="0" sqref="A8"/>
+      <selection pane="bottomRight" activeCell="C17" activeCellId="0" sqref="C17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="1" width="12.15"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="1" width="17.36"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="1" width="32.82"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="1" width="24.14"/>
-    <col collapsed="false" customWidth="false" hidden="true" outlineLevel="0" max="4" min="4" style="1" width="11.52"/>
-    <col collapsed="false" customWidth="true" hidden="true" outlineLevel="0" max="5" min="5" style="1" width="52.27"/>
-    <col collapsed="false" customWidth="false" hidden="true" outlineLevel="0" max="7" min="6" style="1" width="11.52"/>
-    <col collapsed="false" customWidth="true" hidden="true" outlineLevel="0" max="8" min="8" style="1" width="20.31"/>
-    <col collapsed="false" customWidth="true" hidden="true" outlineLevel="0" max="9" min="9" style="1" width="29.18"/>
-    <col collapsed="false" customWidth="true" hidden="true" outlineLevel="0" max="10" min="10" style="1" width="25.52"/>
-    <col collapsed="false" customWidth="false" hidden="false" outlineLevel="0" max="12" min="11" style="1" width="11.52"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="13" min="13" style="1" width="23.8"/>
-    <col collapsed="false" customWidth="false" hidden="false" outlineLevel="0" max="1025" min="14" style="1" width="11.52"/>
+    <col collapsed="false" customWidth="false" hidden="false" outlineLevel="0" max="4" min="4" style="1" width="11.52"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="5" min="5" style="1" width="52.27"/>
+    <col collapsed="false" customWidth="false" hidden="false" outlineLevel="0" max="8" min="6" style="1" width="11.52"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="9" min="9" style="1" width="20.31"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="10" min="10" style="1" width="29.18"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="11" min="11" style="1" width="25.52"/>
+    <col collapsed="false" customWidth="false" hidden="false" outlineLevel="0" max="13" min="12" style="1" width="11.52"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="14" min="14" style="1" width="23.8"/>
+    <col collapsed="false" customWidth="false" hidden="false" outlineLevel="0" max="1025" min="15" style="1" width="11.52"/>
   </cols>
   <sheetData>
     <row r="1" s="2" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1012,7 +1091,9 @@
       <c r="M1" s="2" t="s">
         <v>12</v>
       </c>
-      <c r="N1" s="3"/>
+      <c r="N1" s="2" t="s">
+        <v>13</v>
+      </c>
       <c r="O1" s="3"/>
       <c r="P1" s="3"/>
       <c r="Q1" s="3"/>
@@ -1052,981 +1133,1046 @@
       <c r="AY1" s="3"/>
       <c r="AZ1" s="3"/>
       <c r="BA1" s="3"/>
-    </row>
-    <row r="2" s="4" customFormat="true" ht="13.1" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="BB1" s="3"/>
+    </row>
+    <row r="2" s="4" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A2" s="4" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
       <c r="B2" s="4" t="s">
-        <v>14</v>
+        <v>15</v>
       </c>
       <c r="C2" s="4" t="s">
-        <v>15</v>
+        <v>16</v>
       </c>
       <c r="E2" s="4" t="s">
-        <v>16</v>
+        <v>17</v>
       </c>
       <c r="F2" s="4" t="s">
-        <v>17</v>
-      </c>
-      <c r="L2" s="4" t="s">
         <v>18</v>
+      </c>
+      <c r="M2" s="4" t="s">
+        <v>19</v>
       </c>
     </row>
     <row r="3" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A3" s="1" t="s">
-        <v>19</v>
+        <v>20</v>
       </c>
       <c r="B3" s="1" t="s">
-        <v>20</v>
+        <v>21</v>
       </c>
       <c r="C3" s="1" t="s">
-        <v>21</v>
+        <v>22</v>
       </c>
       <c r="F3" s="1" t="s">
-        <v>22</v>
+        <v>23</v>
       </c>
     </row>
     <row r="4" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A4" s="1" t="s">
+        <v>20</v>
+      </c>
+      <c r="B4" s="1" t="s">
+        <v>24</v>
+      </c>
+      <c r="C4" s="1" t="s">
+        <v>25</v>
+      </c>
+      <c r="F4" s="1" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="5" s="4" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A5" s="4" t="s">
+        <v>14</v>
+      </c>
+      <c r="B5" s="4" t="s">
         <v>19</v>
       </c>
-      <c r="B4" s="1" t="s">
-        <v>23</v>
-      </c>
-      <c r="C4" s="1" t="s">
-        <v>24</v>
-      </c>
-      <c r="F4" s="1" t="s">
-        <v>22</v>
-      </c>
-    </row>
-    <row r="5" s="4" customFormat="true" ht="13.1" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A5" s="4" t="s">
-        <v>13</v>
-      </c>
-      <c r="B5" s="4" t="s">
-        <v>18</v>
-      </c>
       <c r="C5" s="4" t="s">
-        <v>25</v>
-      </c>
-    </row>
-    <row r="6" s="4" customFormat="true" ht="13.1" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="6" s="4" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A6" s="5" t="s">
-        <v>26</v>
-      </c>
-    </row>
-    <row r="7" s="4" customFormat="true" ht="13.1" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="7" s="4" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A7" s="4" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
       <c r="B7" s="4" t="s">
-        <v>27</v>
+        <v>28</v>
       </c>
       <c r="C7" s="4" t="s">
-        <v>28</v>
+        <v>29</v>
       </c>
     </row>
     <row r="8" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A8" s="6" t="s">
-        <v>29</v>
+        <v>30</v>
       </c>
       <c r="B8" s="1" t="s">
-        <v>30</v>
+        <v>31</v>
       </c>
       <c r="C8" s="1" t="s">
-        <v>30</v>
+        <v>31</v>
       </c>
       <c r="F8" s="1" t="s">
-        <v>22</v>
-      </c>
-    </row>
-    <row r="9" s="4" customFormat="true" ht="13.1" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A9" s="5" t="s">
-        <v>26</v>
-      </c>
-    </row>
-    <row r="10" s="4" customFormat="true" ht="13.1" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="9" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A9" s="6" t="s">
+        <v>20</v>
+      </c>
+      <c r="B9" s="1" t="s">
+        <v>32</v>
+      </c>
+      <c r="C9" s="1" t="s">
+        <v>33</v>
+      </c>
+      <c r="F9" s="1" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="10" s="4" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A10" s="5" t="s">
-        <v>26</v>
-      </c>
-    </row>
-    <row r="11" customFormat="false" ht="23.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A11" s="7" t="s">
-        <v>31</v>
-      </c>
-      <c r="B11" s="1" t="s">
-        <v>32</v>
-      </c>
-      <c r="C11" s="1" t="s">
-        <v>33</v>
-      </c>
-      <c r="I11" s="1" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="11" s="4" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A11" s="5" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="12" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A12" s="7" t="s">
         <v>34</v>
       </c>
-    </row>
-    <row r="12" s="4" customFormat="true" ht="13.1" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A12" s="4" t="s">
-        <v>13</v>
-      </c>
-      <c r="B12" s="4" t="s">
+      <c r="B12" s="1" t="s">
         <v>35</v>
       </c>
-      <c r="C12" s="4" t="s">
+      <c r="C12" s="1" t="s">
         <v>36</v>
       </c>
-      <c r="F12" s="4" t="s">
-        <v>17</v>
-      </c>
-    </row>
-    <row r="13" customFormat="false" ht="13.1" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A13" s="1" t="s">
+      <c r="J12" s="1" t="s">
         <v>37</v>
+      </c>
+    </row>
+    <row r="13" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A13" s="7" t="s">
+        <v>34</v>
       </c>
       <c r="B13" s="1" t="s">
         <v>38</v>
       </c>
       <c r="C13" s="1" t="s">
+        <v>33</v>
+      </c>
+      <c r="J13" s="1" t="s">
         <v>39</v>
       </c>
     </row>
-    <row r="14" customFormat="false" ht="46.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A14" s="1" t="s">
-        <v>37</v>
-      </c>
-      <c r="B14" s="1" t="s">
+    <row r="14" s="4" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A14" s="4" t="s">
+        <v>14</v>
+      </c>
+      <c r="B14" s="4" t="s">
         <v>40</v>
       </c>
-      <c r="C14" s="1" t="s">
+      <c r="C14" s="4" t="s">
         <v>41</v>
       </c>
-    </row>
-    <row r="15" s="4" customFormat="true" ht="13.1" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A15" s="5" t="s">
-        <v>26</v>
-      </c>
-    </row>
-    <row r="16" s="4" customFormat="true" ht="13.1" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A16" s="4" t="s">
-        <v>13</v>
-      </c>
-      <c r="B16" s="4" t="s">
-        <v>42</v>
-      </c>
-      <c r="C16" s="4" t="s">
+      <c r="F14" s="4" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="15" customFormat="false" ht="35.05" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A15" s="1" t="s">
+        <v>42</v>
+      </c>
+      <c r="B15" s="1" t="s">
         <v>43</v>
       </c>
-      <c r="F16" s="4" t="s">
-        <v>17</v>
-      </c>
-    </row>
-    <row r="17" customFormat="false" ht="57.45" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="C15" s="1" t="s">
+        <v>44</v>
+      </c>
+    </row>
+    <row r="16" customFormat="false" ht="91" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A16" s="1" t="s">
+        <v>42</v>
+      </c>
+      <c r="B16" s="1" t="s">
+        <v>45</v>
+      </c>
+      <c r="C16" s="1" t="s">
+        <v>46</v>
+      </c>
+      <c r="F16" s="0"/>
+      <c r="G16" s="8" t="s">
+        <v>47</v>
+      </c>
+    </row>
+    <row r="17" customFormat="false" ht="46.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A17" s="1" t="s">
-        <v>37</v>
+        <v>42</v>
       </c>
       <c r="B17" s="1" t="s">
-        <v>44</v>
+        <v>48</v>
       </c>
       <c r="C17" s="1" t="s">
-        <v>45</v>
-      </c>
-      <c r="M17" s="0"/>
+        <v>49</v>
+      </c>
     </row>
     <row r="18" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A18" s="1" t="s">
-        <v>37</v>
+        <v>42</v>
       </c>
       <c r="B18" s="1" t="s">
-        <v>46</v>
-      </c>
-      <c r="M18" s="0" t="s">
-        <v>47</v>
-      </c>
-    </row>
-    <row r="19" s="4" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A19" s="5" t="s">
-        <v>26</v>
-      </c>
-    </row>
-    <row r="20" s="4" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A20" s="4" t="s">
-        <v>13</v>
-      </c>
-      <c r="B20" s="4" t="s">
-        <v>48</v>
-      </c>
-      <c r="C20" s="4" t="s">
-        <v>49</v>
-      </c>
-      <c r="F20" s="4" t="s">
-        <v>17</v>
-      </c>
-    </row>
-    <row r="21" customFormat="false" ht="68.65" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+        <v>50</v>
+      </c>
+      <c r="C18" s="1" t="s">
+        <v>51</v>
+      </c>
+    </row>
+    <row r="19" customFormat="false" ht="23.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A19" s="1" t="s">
+        <v>42</v>
+      </c>
+      <c r="B19" s="1" t="s">
+        <v>52</v>
+      </c>
+      <c r="C19" s="1" t="s">
+        <v>53</v>
+      </c>
+    </row>
+    <row r="20" customFormat="false" ht="46.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A20" s="1" t="s">
+        <v>42</v>
+      </c>
+      <c r="B20" s="1" t="s">
+        <v>54</v>
+      </c>
+      <c r="C20" s="1" t="s">
+        <v>55</v>
+      </c>
+    </row>
+    <row r="21" customFormat="false" ht="23.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A21" s="1" t="s">
-        <v>37</v>
+        <v>42</v>
       </c>
       <c r="B21" s="1" t="s">
-        <v>50</v>
-      </c>
-      <c r="C21" s="8" t="s">
-        <v>51</v>
-      </c>
-    </row>
-    <row r="22" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+        <v>56</v>
+      </c>
+      <c r="C21" s="1" t="s">
+        <v>57</v>
+      </c>
+    </row>
+    <row r="22" customFormat="false" ht="23.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A22" s="1" t="s">
-        <v>37</v>
+        <v>42</v>
       </c>
       <c r="B22" s="1" t="s">
-        <v>52</v>
-      </c>
-      <c r="C22" s="8"/>
-      <c r="M22" s="1" t="s">
-        <v>53</v>
-      </c>
-    </row>
-    <row r="23" s="4" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A23" s="5" t="s">
-        <v>26</v>
+        <v>58</v>
+      </c>
+      <c r="C22" s="1" t="s">
+        <v>59</v>
+      </c>
+    </row>
+    <row r="23" customFormat="false" ht="46.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A23" s="1" t="s">
+        <v>42</v>
+      </c>
+      <c r="B23" s="1" t="s">
+        <v>60</v>
+      </c>
+      <c r="C23" s="1" t="s">
+        <v>61</v>
       </c>
     </row>
     <row r="24" s="4" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A24" s="4" t="s">
-        <v>13</v>
-      </c>
-      <c r="B24" s="4" t="s">
-        <v>54</v>
-      </c>
-      <c r="C24" s="4" t="s">
-        <v>55</v>
-      </c>
-      <c r="F24" s="4" t="s">
-        <v>17</v>
-      </c>
-    </row>
-    <row r="25" customFormat="false" ht="35.05" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A25" s="1" t="s">
-        <v>37</v>
-      </c>
-      <c r="B25" s="1" t="s">
-        <v>56</v>
-      </c>
-      <c r="C25" s="8" t="s">
-        <v>57</v>
-      </c>
-    </row>
-    <row r="26" customFormat="false" ht="46.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A24" s="5" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="25" s="4" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A25" s="4" t="s">
+        <v>14</v>
+      </c>
+      <c r="B25" s="4" t="s">
+        <v>62</v>
+      </c>
+      <c r="C25" s="4" t="s">
+        <v>63</v>
+      </c>
+      <c r="F25" s="4" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="26" customFormat="false" ht="57.45" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A26" s="1" t="s">
-        <v>37</v>
+        <v>42</v>
       </c>
       <c r="B26" s="1" t="s">
-        <v>58</v>
-      </c>
-      <c r="C26" s="8" t="s">
-        <v>59</v>
-      </c>
+        <v>64</v>
+      </c>
+      <c r="C26" s="1" t="s">
+        <v>65</v>
+      </c>
+      <c r="N26" s="0"/>
     </row>
     <row r="27" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A27" s="1" t="s">
-        <v>37</v>
+        <v>42</v>
       </c>
       <c r="B27" s="1" t="s">
-        <v>60</v>
-      </c>
-      <c r="C27" s="8"/>
-      <c r="M27" s="1" t="s">
-        <v>61</v>
+        <v>66</v>
+      </c>
+      <c r="N27" s="0" t="s">
+        <v>67</v>
       </c>
     </row>
     <row r="28" s="4" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A28" s="5" t="s">
-        <v>26</v>
+        <v>27</v>
       </c>
     </row>
     <row r="29" s="4" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A29" s="4" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
       <c r="B29" s="4" t="s">
-        <v>62</v>
+        <v>68</v>
       </c>
       <c r="C29" s="4" t="s">
-        <v>63</v>
+        <v>69</v>
       </c>
       <c r="F29" s="4" t="s">
-        <v>17</v>
-      </c>
-    </row>
-    <row r="30" customFormat="false" ht="57.45" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="30" customFormat="false" ht="68.65" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A30" s="1" t="s">
-        <v>37</v>
+        <v>42</v>
       </c>
       <c r="B30" s="1" t="s">
-        <v>64</v>
-      </c>
-      <c r="C30" s="8" t="s">
-        <v>65</v>
+        <v>70</v>
+      </c>
+      <c r="C30" s="9" t="s">
+        <v>71</v>
       </c>
     </row>
     <row r="31" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A31" s="1" t="s">
-        <v>37</v>
+        <v>42</v>
       </c>
       <c r="B31" s="1" t="s">
-        <v>66</v>
-      </c>
-      <c r="C31" s="8"/>
-      <c r="M31" s="1" t="s">
-        <v>67</v>
-      </c>
-    </row>
-    <row r="32" s="4" customFormat="true" ht="13.1" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+        <v>72</v>
+      </c>
+      <c r="C31" s="9"/>
+      <c r="N31" s="1" t="s">
+        <v>73</v>
+      </c>
+    </row>
+    <row r="32" s="4" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A32" s="5" t="s">
-        <v>26</v>
-      </c>
-    </row>
-    <row r="33" s="4" customFormat="true" ht="13.1" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="33" s="4" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A33" s="4" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
       <c r="B33" s="4" t="s">
-        <v>68</v>
+        <v>74</v>
       </c>
       <c r="C33" s="4" t="s">
-        <v>69</v>
+        <v>75</v>
       </c>
       <c r="F33" s="4" t="s">
-        <v>17</v>
-      </c>
-    </row>
-    <row r="34" customFormat="false" ht="68.65" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="34" customFormat="false" ht="35.05" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A34" s="1" t="s">
-        <v>37</v>
+        <v>42</v>
       </c>
       <c r="B34" s="1" t="s">
-        <v>70</v>
-      </c>
-      <c r="C34" s="8" t="s">
-        <v>71</v>
-      </c>
-    </row>
-    <row r="35" customFormat="false" ht="23.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+        <v>76</v>
+      </c>
+      <c r="C34" s="9" t="s">
+        <v>77</v>
+      </c>
+    </row>
+    <row r="35" customFormat="false" ht="46.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A35" s="1" t="s">
-        <v>37</v>
+        <v>42</v>
       </c>
       <c r="B35" s="1" t="s">
-        <v>72</v>
-      </c>
-      <c r="C35" s="8"/>
-      <c r="M35" s="1" t="s">
-        <v>73</v>
-      </c>
-    </row>
-    <row r="36" s="4" customFormat="true" ht="13.1" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A36" s="5" t="s">
-        <v>26</v>
-      </c>
-    </row>
-    <row r="37" s="4" customFormat="true" ht="13.1" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A37" s="4" t="s">
-        <v>13</v>
-      </c>
-      <c r="B37" s="4" t="s">
-        <v>74</v>
-      </c>
-      <c r="C37" s="4" t="s">
-        <v>75</v>
-      </c>
-      <c r="F37" s="4" t="s">
-        <v>17</v>
-      </c>
-    </row>
-    <row r="38" customFormat="false" ht="35.05" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A38" s="1" t="s">
-        <v>37</v>
-      </c>
-      <c r="B38" s="1" t="s">
-        <v>76</v>
-      </c>
-      <c r="C38" s="1" t="s">
-        <v>77</v>
-      </c>
-    </row>
-    <row r="39" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+        <v>78</v>
+      </c>
+      <c r="C35" s="9" t="s">
+        <v>79</v>
+      </c>
+    </row>
+    <row r="36" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A36" s="1" t="s">
+        <v>42</v>
+      </c>
+      <c r="B36" s="1" t="s">
+        <v>80</v>
+      </c>
+      <c r="C36" s="9"/>
+      <c r="N36" s="1" t="s">
+        <v>81</v>
+      </c>
+    </row>
+    <row r="37" s="4" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A37" s="5" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="38" s="4" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A38" s="4" t="s">
+        <v>14</v>
+      </c>
+      <c r="B38" s="4" t="s">
+        <v>82</v>
+      </c>
+      <c r="C38" s="4" t="s">
+        <v>83</v>
+      </c>
+      <c r="F38" s="4" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="39" customFormat="false" ht="57.45" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A39" s="1" t="s">
-        <v>37</v>
+        <v>42</v>
       </c>
       <c r="B39" s="1" t="s">
-        <v>78</v>
-      </c>
-      <c r="M39" s="1" t="s">
-        <v>79</v>
-      </c>
-    </row>
-    <row r="40" s="4" customFormat="true" ht="13.1" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A40" s="5" t="s">
-        <v>26</v>
-      </c>
-    </row>
-    <row r="41" s="4" customFormat="true" ht="13.1" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A41" s="4" t="s">
-        <v>13</v>
-      </c>
-      <c r="B41" s="4" t="s">
-        <v>80</v>
-      </c>
-      <c r="C41" s="4" t="s">
-        <v>81</v>
-      </c>
-      <c r="F41" s="4" t="s">
-        <v>17</v>
-      </c>
-    </row>
-    <row r="42" customFormat="false" ht="35.05" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A42" s="1" t="s">
-        <v>82</v>
-      </c>
-      <c r="B42" s="1" t="s">
-        <v>83</v>
-      </c>
-      <c r="C42" s="1" t="s">
         <v>84</v>
       </c>
-      <c r="D42" s="1" t="s">
+      <c r="C39" s="9" t="s">
         <v>85</v>
       </c>
     </row>
-    <row r="43" customFormat="false" ht="79.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A43" s="7" t="s">
-        <v>31</v>
+    <row r="40" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A40" s="1" t="s">
+        <v>42</v>
+      </c>
+      <c r="B40" s="1" t="s">
+        <v>86</v>
+      </c>
+      <c r="C40" s="9"/>
+      <c r="N40" s="1" t="s">
+        <v>87</v>
+      </c>
+    </row>
+    <row r="41" s="4" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A41" s="5" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="42" s="4" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A42" s="4" t="s">
+        <v>14</v>
+      </c>
+      <c r="B42" s="4" t="s">
+        <v>88</v>
+      </c>
+      <c r="C42" s="4" t="s">
+        <v>89</v>
+      </c>
+      <c r="F42" s="4" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="43" customFormat="false" ht="68.65" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A43" s="1" t="s">
+        <v>42</v>
       </c>
       <c r="B43" s="1" t="s">
-        <v>86</v>
-      </c>
-      <c r="C43" s="1" t="s">
-        <v>87</v>
-      </c>
-      <c r="I43" s="1" t="s">
-        <v>88</v>
-      </c>
-    </row>
-    <row r="44" customFormat="false" ht="35.05" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+        <v>90</v>
+      </c>
+      <c r="C43" s="9" t="s">
+        <v>91</v>
+      </c>
+    </row>
+    <row r="44" customFormat="false" ht="23.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A44" s="1" t="s">
-        <v>89</v>
+        <v>42</v>
       </c>
       <c r="B44" s="1" t="s">
-        <v>90</v>
-      </c>
-      <c r="C44" s="1" t="s">
-        <v>91</v>
-      </c>
-      <c r="D44" s="1" t="s">
-        <v>85</v>
-      </c>
-    </row>
-    <row r="45" customFormat="false" ht="68.65" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A45" s="7" t="s">
-        <v>31</v>
-      </c>
-      <c r="B45" s="1" t="s">
         <v>92</v>
       </c>
-      <c r="C45" s="1" t="s">
-        <v>87</v>
-      </c>
-      <c r="I45" s="1" t="s">
+      <c r="C44" s="9"/>
+      <c r="N44" s="1" t="s">
         <v>93</v>
       </c>
     </row>
-    <row r="46" customFormat="false" ht="35.05" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A46" s="1" t="s">
+    <row r="45" s="4" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A45" s="5" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="46" s="4" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A46" s="4" t="s">
+        <v>14</v>
+      </c>
+      <c r="B46" s="4" t="s">
         <v>94</v>
       </c>
-      <c r="B46" s="1" t="s">
+      <c r="C46" s="4" t="s">
         <v>95</v>
       </c>
-      <c r="C46" s="1" t="s">
+      <c r="F46" s="4" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="47" customFormat="false" ht="35.05" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A47" s="1" t="s">
+        <v>42</v>
+      </c>
+      <c r="B47" s="1" t="s">
         <v>96</v>
       </c>
-      <c r="D46" s="1" t="s">
-        <v>85</v>
-      </c>
-    </row>
-    <row r="47" customFormat="false" ht="79.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A47" s="7" t="s">
-        <v>31</v>
-      </c>
-      <c r="B47" s="1" t="s">
+      <c r="C47" s="1" t="s">
         <v>97</v>
       </c>
-      <c r="C47" s="1" t="s">
-        <v>87</v>
-      </c>
-      <c r="I47" s="1" t="s">
+    </row>
+    <row r="48" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A48" s="1" t="s">
+        <v>42</v>
+      </c>
+      <c r="B48" s="1" t="s">
         <v>98</v>
       </c>
-    </row>
-    <row r="48" customFormat="false" ht="46.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A48" s="1" t="s">
+      <c r="N48" s="1" t="s">
         <v>99</v>
       </c>
-      <c r="B48" s="1" t="s">
+    </row>
+    <row r="49" s="4" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A49" s="5" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="50" s="4" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A50" s="4" t="s">
+        <v>14</v>
+      </c>
+      <c r="B50" s="4" t="s">
         <v>100</v>
       </c>
-      <c r="C48" s="1" t="s">
+      <c r="C50" s="4" t="s">
         <v>101</v>
       </c>
-      <c r="D48" s="1" t="s">
-        <v>85</v>
-      </c>
-    </row>
-    <row r="49" customFormat="false" ht="57.45" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A49" s="7" t="s">
-        <v>31</v>
-      </c>
-      <c r="B49" s="1" t="s">
+      <c r="F50" s="4" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="51" customFormat="false" ht="35.05" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A51" s="1" t="s">
         <v>102</v>
       </c>
-      <c r="C49" s="1" t="s">
-        <v>87</v>
-      </c>
-      <c r="I49" s="1" t="s">
+      <c r="B51" s="1" t="s">
         <v>103</v>
       </c>
-    </row>
-    <row r="50" customFormat="false" ht="46.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A50" s="1" t="s">
+      <c r="C51" s="1" t="s">
         <v>104</v>
       </c>
-      <c r="B50" s="1" t="s">
+      <c r="D51" s="1" t="s">
         <v>105</v>
       </c>
-      <c r="C50" s="1" t="s">
+    </row>
+    <row r="52" customFormat="false" ht="35.05" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A52" s="7" t="s">
+        <v>34</v>
+      </c>
+      <c r="B52" s="1" t="s">
         <v>106</v>
       </c>
-      <c r="D50" s="1" t="s">
-        <v>85</v>
-      </c>
-    </row>
-    <row r="51" customFormat="false" ht="57.45" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A51" s="7" t="s">
-        <v>31</v>
-      </c>
-      <c r="B51" s="1" t="s">
+      <c r="C52" s="1" t="s">
         <v>107</v>
       </c>
-      <c r="C51" s="1" t="s">
-        <v>87</v>
-      </c>
-      <c r="I51" s="1" t="s">
+      <c r="J52" s="1" t="s">
         <v>108</v>
       </c>
     </row>
-    <row r="52" s="4" customFormat="true" ht="13.1" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A52" s="5" t="s">
-        <v>26</v>
-      </c>
-    </row>
-    <row r="53" customFormat="false" ht="57.45" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A53" s="7" t="s">
-        <v>31</v>
+    <row r="53" customFormat="false" ht="35.05" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A53" s="1" t="s">
+        <v>109</v>
       </c>
       <c r="B53" s="1" t="s">
-        <v>109</v>
-      </c>
-      <c r="I53" s="1" t="s">
         <v>110</v>
+      </c>
+      <c r="C53" s="1" t="s">
+        <v>111</v>
+      </c>
+      <c r="D53" s="1" t="s">
+        <v>105</v>
       </c>
     </row>
     <row r="54" customFormat="false" ht="23.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A54" s="7" t="s">
-        <v>31</v>
+        <v>34</v>
       </c>
       <c r="B54" s="1" t="s">
-        <v>111</v>
-      </c>
-      <c r="I54" s="1" t="s">
         <v>112</v>
       </c>
-    </row>
-    <row r="55" s="4" customFormat="true" ht="23.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A55" s="4" t="s">
-        <v>13</v>
-      </c>
-      <c r="B55" s="4" t="s">
+      <c r="C54" s="1" t="s">
+        <v>107</v>
+      </c>
+      <c r="J54" s="1" t="s">
         <v>113</v>
       </c>
-      <c r="C55" s="4" t="s">
-        <v>87</v>
-      </c>
-      <c r="F55" s="4" t="s">
+    </row>
+    <row r="55" customFormat="false" ht="23.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A55" s="1" t="s">
         <v>114</v>
       </c>
-    </row>
-    <row r="56" customFormat="false" ht="13.1" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A56" s="1" t="s">
-        <v>37</v>
+      <c r="B55" s="1" t="s">
+        <v>115</v>
+      </c>
+      <c r="C55" s="1" t="s">
+        <v>116</v>
+      </c>
+      <c r="D55" s="1" t="s">
+        <v>105</v>
+      </c>
+    </row>
+    <row r="56" customFormat="false" ht="35.05" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A56" s="7" t="s">
+        <v>34</v>
       </c>
       <c r="B56" s="1" t="s">
-        <v>115</v>
+        <v>117</v>
       </c>
       <c r="C56" s="1" t="s">
-        <v>116</v>
-      </c>
-    </row>
-    <row r="57" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+        <v>107</v>
+      </c>
+      <c r="J56" s="1" t="s">
+        <v>118</v>
+      </c>
+    </row>
+    <row r="57" customFormat="false" ht="46.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A57" s="1" t="s">
-        <v>37</v>
+        <v>119</v>
       </c>
       <c r="B57" s="1" t="s">
-        <v>117</v>
+        <v>120</v>
       </c>
       <c r="C57" s="1" t="s">
-        <v>118</v>
-      </c>
-      <c r="F57" s="1" t="s">
-        <v>119</v>
-      </c>
-    </row>
-    <row r="58" customFormat="false" ht="46.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A58" s="1" t="s">
-        <v>37</v>
+        <v>121</v>
+      </c>
+      <c r="D57" s="1" t="s">
+        <v>105</v>
+      </c>
+    </row>
+    <row r="58" customFormat="false" ht="23.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A58" s="7" t="s">
+        <v>34</v>
       </c>
       <c r="B58" s="1" t="s">
-        <v>120</v>
+        <v>122</v>
       </c>
       <c r="C58" s="1" t="s">
-        <v>121</v>
-      </c>
-      <c r="E58" s="1" t="s">
-        <v>122</v>
-      </c>
-    </row>
-    <row r="59" customFormat="false" ht="35.6" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+        <v>107</v>
+      </c>
+      <c r="J58" s="1" t="s">
+        <v>123</v>
+      </c>
+    </row>
+    <row r="59" customFormat="false" ht="46.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A59" s="1" t="s">
-        <v>37</v>
+        <v>124</v>
       </c>
       <c r="B59" s="1" t="s">
-        <v>123</v>
+        <v>125</v>
       </c>
       <c r="C59" s="1" t="s">
-        <v>124</v>
-      </c>
-      <c r="E59" s="1" t="s">
-        <v>122</v>
-      </c>
-    </row>
-    <row r="60" customFormat="false" ht="46.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A60" s="1" t="s">
-        <v>37</v>
+        <v>126</v>
+      </c>
+      <c r="D59" s="1" t="s">
+        <v>105</v>
+      </c>
+    </row>
+    <row r="60" customFormat="false" ht="23.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A60" s="7" t="s">
+        <v>34</v>
       </c>
       <c r="B60" s="1" t="s">
-        <v>125</v>
+        <v>127</v>
       </c>
       <c r="C60" s="1" t="s">
-        <v>126</v>
-      </c>
-      <c r="E60" s="1" t="s">
-        <v>127</v>
-      </c>
-    </row>
-    <row r="61" customFormat="false" ht="35.6" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A61" s="1" t="s">
-        <v>37</v>
-      </c>
-      <c r="B61" s="1" t="s">
+        <v>107</v>
+      </c>
+      <c r="J60" s="1" t="s">
         <v>128</v>
       </c>
-      <c r="C61" s="1" t="s">
+    </row>
+    <row r="61" s="4" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A61" s="5" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="62" customFormat="false" ht="57.45" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A62" s="7" t="s">
+        <v>34</v>
+      </c>
+      <c r="B62" s="1" t="s">
         <v>129</v>
       </c>
-      <c r="E61" s="1" t="s">
-        <v>127</v>
-      </c>
-    </row>
-    <row r="62" customFormat="false" ht="23.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A62" s="1" t="s">
-        <v>37</v>
-      </c>
-      <c r="B62" s="1" t="s">
+      <c r="J62" s="1" t="s">
         <v>130</v>
       </c>
-      <c r="C62" s="1" t="s">
+    </row>
+    <row r="63" customFormat="false" ht="23.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A63" s="7" t="s">
+        <v>34</v>
+      </c>
+      <c r="B63" s="1" t="s">
         <v>131</v>
       </c>
-      <c r="E62" s="1" t="s">
-        <v>127</v>
-      </c>
-    </row>
-    <row r="63" customFormat="false" ht="23.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A63" s="1" t="s">
-        <v>37</v>
-      </c>
-      <c r="B63" s="1" t="s">
+      <c r="J63" s="1" t="s">
         <v>132</v>
       </c>
-      <c r="C63" s="1" t="s">
+    </row>
+    <row r="64" s="4" customFormat="true" ht="23.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A64" s="4" t="s">
+        <v>14</v>
+      </c>
+      <c r="B64" s="4" t="s">
         <v>133</v>
       </c>
-      <c r="E63" s="1" t="s">
+      <c r="C64" s="4" t="s">
+        <v>107</v>
+      </c>
+      <c r="F64" s="4" t="s">
         <v>134</v>
       </c>
-      <c r="F63" s="1" t="s">
+    </row>
+    <row r="65" customFormat="false" ht="46.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A65" s="1" t="s">
+        <v>42</v>
+      </c>
+      <c r="B65" s="1" t="s">
         <v>135</v>
       </c>
-    </row>
-    <row r="64" customFormat="false" ht="23.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A64" s="1" t="s">
-        <v>37</v>
-      </c>
-      <c r="B64" s="1" t="s">
+      <c r="C65" s="1" t="s">
         <v>136</v>
-      </c>
-      <c r="C64" s="1" t="s">
-        <v>137</v>
-      </c>
-      <c r="E64" s="1" t="s">
-        <v>138</v>
-      </c>
-      <c r="F64" s="1" t="s">
-        <v>135</v>
-      </c>
-    </row>
-    <row r="65" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A65" s="1" t="s">
-        <v>37</v>
-      </c>
-      <c r="B65" s="1" t="s">
-        <v>139</v>
-      </c>
-      <c r="C65" s="1" t="s">
-        <v>69</v>
-      </c>
-      <c r="E65" s="1" t="s">
-        <v>140</v>
-      </c>
-      <c r="F65" s="1" t="s">
-        <v>135</v>
       </c>
     </row>
     <row r="66" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A66" s="1" t="s">
-        <v>37</v>
+        <v>42</v>
       </c>
       <c r="B66" s="1" t="s">
+        <v>137</v>
+      </c>
+      <c r="C66" s="1" t="s">
+        <v>138</v>
+      </c>
+      <c r="F66" s="1" t="s">
+        <v>139</v>
+      </c>
+    </row>
+    <row r="67" customFormat="false" ht="46.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A67" s="1" t="s">
+        <v>42</v>
+      </c>
+      <c r="B67" s="1" t="s">
+        <v>140</v>
+      </c>
+      <c r="C67" s="1" t="s">
         <v>141</v>
       </c>
-      <c r="C66" s="1" t="s">
+      <c r="E67" s="1" t="s">
         <v>142</v>
       </c>
-      <c r="E66" s="1" t="s">
+    </row>
+    <row r="68" customFormat="false" ht="23.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A68" s="1" t="s">
         <v>143</v>
       </c>
-      <c r="F66" s="1" t="s">
-        <v>135</v>
-      </c>
-    </row>
-    <row r="67" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A67" s="1" t="s">
-        <v>37</v>
-      </c>
-      <c r="B67" s="1" t="s">
+      <c r="B68" s="1" t="s">
         <v>144</v>
       </c>
-      <c r="C67" s="1" t="s">
+      <c r="C68" s="1" t="s">
         <v>145</v>
       </c>
-      <c r="E67" s="1" t="s">
+      <c r="D68" s="1" t="s">
+        <v>105</v>
+      </c>
+      <c r="E68" s="1" t="s">
+        <v>142</v>
+      </c>
+    </row>
+    <row r="69" customFormat="false" ht="23.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A69" s="1" t="s">
         <v>146</v>
       </c>
-      <c r="F67" s="1" t="s">
-        <v>135</v>
-      </c>
-    </row>
-    <row r="68" customFormat="false" ht="35.05" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A68" s="1" t="s">
-        <v>37</v>
-      </c>
-      <c r="B68" s="1" t="s">
+      <c r="B69" s="1" t="s">
         <v>147</v>
       </c>
-      <c r="C68" s="1" t="s">
+      <c r="C69" s="1" t="s">
         <v>148</v>
       </c>
-      <c r="E68" s="1" t="s">
-        <v>127</v>
-      </c>
-    </row>
-    <row r="69" s="4" customFormat="true" ht="13.1" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A69" s="5" t="s">
-        <v>26</v>
+      <c r="D69" s="1" t="s">
+        <v>105</v>
+      </c>
+      <c r="E69" s="1" t="s">
+        <v>142</v>
+      </c>
+    </row>
+    <row r="70" customFormat="false" ht="35.05" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A70" s="1" t="s">
+        <v>149</v>
+      </c>
+      <c r="B70" s="1" t="s">
+        <v>150</v>
+      </c>
+      <c r="C70" s="1" t="s">
+        <v>151</v>
+      </c>
+      <c r="E70" s="1" t="s">
+        <v>142</v>
+      </c>
+      <c r="L70" s="1" t="s">
+        <v>152</v>
+      </c>
+    </row>
+    <row r="71" customFormat="false" ht="46.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A71" s="1" t="s">
+        <v>42</v>
+      </c>
+      <c r="B71" s="1" t="s">
+        <v>153</v>
+      </c>
+      <c r="C71" s="1" t="s">
+        <v>154</v>
+      </c>
+      <c r="E71" s="1" t="s">
+        <v>155</v>
+      </c>
+    </row>
+    <row r="72" customFormat="false" ht="35.05" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A72" s="1" t="s">
+        <v>42</v>
+      </c>
+      <c r="B72" s="1" t="s">
+        <v>156</v>
+      </c>
+      <c r="C72" s="1" t="s">
+        <v>157</v>
+      </c>
+      <c r="E72" s="1" t="s">
+        <v>155</v>
+      </c>
+    </row>
+    <row r="73" customFormat="false" ht="57.45" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A73" s="1" t="s">
+        <v>42</v>
+      </c>
+      <c r="B73" s="1" t="s">
+        <v>158</v>
+      </c>
+      <c r="C73" s="1" t="s">
+        <v>159</v>
+      </c>
+      <c r="E73" s="1" t="s">
+        <v>155</v>
+      </c>
+    </row>
+    <row r="74" customFormat="false" ht="23.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A74" s="1" t="s">
+        <v>146</v>
+      </c>
+      <c r="B74" s="1" t="s">
+        <v>160</v>
+      </c>
+      <c r="C74" s="1" t="s">
+        <v>161</v>
+      </c>
+      <c r="E74" s="1" t="s">
+        <v>155</v>
+      </c>
+      <c r="L74" s="1" t="s">
+        <v>162</v>
+      </c>
+    </row>
+    <row r="75" s="4" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A75" s="5" t="s">
+        <v>27</v>
       </c>
     </row>
   </sheetData>
-  <conditionalFormatting sqref="C21:C22">
+  <conditionalFormatting sqref="C30:C31">
     <cfRule type="containsText" priority="2" operator="containsText" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="calculate" dxfId="0"/>
   </conditionalFormatting>
-  <conditionalFormatting sqref="C21:C22">
+  <conditionalFormatting sqref="C30:C31">
     <cfRule type="expression" priority="3" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="1">
-      <formula>AND($A21="begin group", NOT($B21 = ""))</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="C21:C22">
+      <formula>AND($A30="begin group", NOT($B30 = ""))</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="C30:C31">
     <cfRule type="expression" priority="4" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="2">
-      <formula>AND($A21="end group", $B21 = "", $C21 = "", $D21 = "", $E21 = "", $F21 = "", $G21 = "", $H21 = "", $I21 = "", $J21 = "", $K21 = "", $L21 = "", $M21 = "")</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="C21:C22">
+      <formula>AND($A30="end group", $B30 = "", $C30 = "", $D30 = "", $E30 = "", $F30 = "", $H30 = "", $I30 = "", $J30 = "", $K30 = "", $L30 = "", $M30 = "", $N30 = "")</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="C30:C31">
     <cfRule type="cellIs" priority="5" operator="equal" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="3">
       <formula>"note"</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="C21:C22">
+  <conditionalFormatting sqref="C30:C31">
     <cfRule type="expression" priority="6" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="4">
-      <formula>AND(AND(NOT($A21 = "end group"), NOT($A21 = "end repeat"), NOT($A21 = "")), $C21 = "")</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="C21:C22">
+      <formula>AND(AND(NOT($A30 = "end group"), NOT($A30 = "end repeat"), NOT($A30 = "")), $C30 = "")</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="C30:C31">
     <cfRule type="expression" priority="7" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="5">
-      <formula>AND($A21="begin repeat", NOT($B21 = ""))</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="C21:C22">
+      <formula>AND($A30="begin repeat", NOT($B30 = ""))</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="C30:C31">
     <cfRule type="expression" priority="8" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="6">
-      <formula>AND($A21="end repeat", $B21 = "", $C21 = "", $D21 = "", $E21 = "", $F21 = "", $G21 = "", $H21 = "", $I21 = "", $J21 = "", $K21 = "", $L21 = "", $M21 = "")</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="C25">
+      <formula>AND($A30="end repeat", $B30 = "", $C30 = "", $D30 = "", $E30 = "", $F30 = "", $H30 = "", $I30 = "", $J30 = "", $K30 = "", $L30 = "", $M30 = "", $N30 = "")</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="C34">
     <cfRule type="containsText" priority="9" operator="containsText" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="calculate" dxfId="0"/>
   </conditionalFormatting>
-  <conditionalFormatting sqref="C25">
+  <conditionalFormatting sqref="C34">
     <cfRule type="expression" priority="10" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="1">
-      <formula>AND($A25="begin group", NOT($B25 = ""))</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="C25">
+      <formula>AND($A34="begin group", NOT($B34 = ""))</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="C34">
     <cfRule type="expression" priority="11" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="2">
-      <formula>AND($A25="end group", $B25 = "", $C25 = "", $D25 = "", $E25 = "", $F25 = "", $G25 = "", $H25 = "", $I25 = "", $J25 = "", $K25 = "", $L25 = "", $M25 = "")</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="C25">
+      <formula>AND($A34="end group", $B34 = "", $C34 = "", $D34 = "", $E34 = "", $F34 = "", $H34 = "", $I34 = "", $J34 = "", $K34 = "", $L34 = "", $M34 = "", $N34 = "")</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="C34">
     <cfRule type="cellIs" priority="12" operator="equal" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="3">
       <formula>"note"</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="C25">
+  <conditionalFormatting sqref="C34">
     <cfRule type="expression" priority="13" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="4">
-      <formula>AND(AND(NOT($A25 = "end group"), NOT($A25 = "end repeat"), NOT($A25 = "")), $C25 = "")</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="C25">
+      <formula>AND(AND(NOT($A34 = "end group"), NOT($A34 = "end repeat"), NOT($A34 = "")), $C34 = "")</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="C34">
     <cfRule type="expression" priority="14" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="5">
-      <formula>AND($A25="begin repeat", NOT($B25 = ""))</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="C25">
+      <formula>AND($A34="begin repeat", NOT($B34 = ""))</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="C34">
     <cfRule type="expression" priority="15" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="6">
-      <formula>AND($A25="end repeat", $B25 = "", $C25 = "", $D25 = "", $E25 = "", $F25 = "", $G25 = "", $H25 = "", $I25 = "", $J25 = "", $K25 = "", $L25 = "", $M25 = "")</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="C26:C27">
+      <formula>AND($A34="end repeat", $B34 = "", $C34 = "", $D34 = "", $E34 = "", $F34 = "", $H34 = "", $I34 = "", $J34 = "", $K34 = "", $L34 = "", $M34 = "", $N34 = "")</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="C35:C36">
     <cfRule type="containsText" priority="16" operator="containsText" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="calculate" dxfId="0"/>
   </conditionalFormatting>
-  <conditionalFormatting sqref="C26:C27">
+  <conditionalFormatting sqref="C35:C36">
     <cfRule type="expression" priority="17" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="1">
-      <formula>AND($A26="begin group", NOT($B26 = ""))</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="C26:C27">
+      <formula>AND($A35="begin group", NOT($B35 = ""))</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="C35:C36">
     <cfRule type="expression" priority="18" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="2">
-      <formula>AND($A26="end group", $B26 = "", $C26 = "", $D26 = "", $E26 = "", $F26 = "", $G26 = "", $H26 = "", $I26 = "", $J26 = "", $K26 = "", $L26 = "", $M26 = "")</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="C26:C27">
+      <formula>AND($A35="end group", $B35 = "", $C35 = "", $D35 = "", $E35 = "", $F35 = "", $H35 = "", $I35 = "", $J35 = "", $K35 = "", $L35 = "", $M35 = "", $N35 = "")</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="C35:C36">
     <cfRule type="cellIs" priority="19" operator="equal" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="3">
       <formula>"note"</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="C26:C27">
+  <conditionalFormatting sqref="C35:C36">
     <cfRule type="expression" priority="20" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="4">
-      <formula>AND(AND(NOT($A26 = "end group"), NOT($A26 = "end repeat"), NOT($A26 = "")), $C26 = "")</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="C26:C27">
+      <formula>AND(AND(NOT($A35 = "end group"), NOT($A35 = "end repeat"), NOT($A35 = "")), $C35 = "")</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="C35:C36">
     <cfRule type="expression" priority="21" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="5">
-      <formula>AND($A26="begin repeat", NOT($B26 = ""))</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="C26:C27">
+      <formula>AND($A35="begin repeat", NOT($B35 = ""))</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="C35:C36">
     <cfRule type="expression" priority="22" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="6">
-      <formula>AND($A26="end repeat", $B26 = "", $C26 = "", $D26 = "", $E26 = "", $F26 = "", $G26 = "", $H26 = "", $I26 = "", $J26 = "", $K26 = "", $L26 = "", $M26 = "")</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="C30:C31">
+      <formula>AND($A35="end repeat", $B35 = "", $C35 = "", $D35 = "", $E35 = "", $F35 = "", $H35 = "", $I35 = "", $J35 = "", $K35 = "", $L35 = "", $M35 = "", $N35 = "")</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="C39:C40">
     <cfRule type="containsText" priority="23" operator="containsText" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="calculate" dxfId="0"/>
   </conditionalFormatting>
-  <conditionalFormatting sqref="C30:C31">
+  <conditionalFormatting sqref="C39:C40">
     <cfRule type="expression" priority="24" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="1">
-      <formula>AND($A30="begin group", NOT($B30 = ""))</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="C30:C31">
+      <formula>AND($A39="begin group", NOT($B39 = ""))</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="C39:C40">
     <cfRule type="expression" priority="25" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="2">
-      <formula>AND($A30="end group", $B30 = "", $C30 = "", $D30 = "", $E30 = "", $F30 = "", $G30 = "", $H30 = "", $I30 = "", $J30 = "", $K30 = "", $L30 = "", $M30 = "")</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="C30:C31">
+      <formula>AND($A39="end group", $B39 = "", $C39 = "", $D39 = "", $E39 = "", $F39 = "", $H39 = "", $I39 = "", $J39 = "", $K39 = "", $L39 = "", $M39 = "", $N39 = "")</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="C39:C40">
     <cfRule type="cellIs" priority="26" operator="equal" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="3">
       <formula>"note"</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="C30:C31">
+  <conditionalFormatting sqref="C39:C40">
     <cfRule type="expression" priority="27" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="4">
-      <formula>AND(AND(NOT($A30 = "end group"), NOT($A30 = "end repeat"), NOT($A30 = "")), $C30 = "")</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="C30:C31">
+      <formula>AND(AND(NOT($A39 = "end group"), NOT($A39 = "end repeat"), NOT($A39 = "")), $C39 = "")</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="C39:C40">
     <cfRule type="expression" priority="28" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="5">
-      <formula>AND($A30="begin repeat", NOT($B30 = ""))</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="C30:C31">
+      <formula>AND($A39="begin repeat", NOT($B39 = ""))</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="C39:C40">
     <cfRule type="expression" priority="29" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="6">
-      <formula>AND($A30="end repeat", $B30 = "", $C30 = "", $D30 = "", $E30 = "", $F30 = "", $G30 = "", $H30 = "", $I30 = "", $J30 = "", $K30 = "", $L30 = "", $M30 = "")</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="C34:C35">
+      <formula>AND($A39="end repeat", $B39 = "", $C39 = "", $D39 = "", $E39 = "", $F39 = "", $H39 = "", $I39 = "", $J39 = "", $K39 = "", $L39 = "", $M39 = "", $N39 = "")</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="C43:C44">
     <cfRule type="containsText" priority="30" operator="containsText" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="calculate" dxfId="0"/>
   </conditionalFormatting>
-  <conditionalFormatting sqref="C34:C35">
+  <conditionalFormatting sqref="C43:C44">
     <cfRule type="expression" priority="31" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="1">
-      <formula>AND($A34="begin group", NOT($B34 = ""))</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="C34:C35">
+      <formula>AND($A43="begin group", NOT($B43 = ""))</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="C43:C44">
     <cfRule type="expression" priority="32" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="2">
-      <formula>AND($A34="end group", $B34 = "", $C34 = "", $D34 = "", $E34 = "", $F34 = "", $G34 = "", $H34 = "", $I34 = "", $J34 = "", $K34 = "", $L34 = "", $M34 = "")</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="C34:C35">
+      <formula>AND($A43="end group", $B43 = "", $C43 = "", $D43 = "", $E43 = "", $F43 = "", $H43 = "", $I43 = "", $J43 = "", $K43 = "", $L43 = "", $M43 = "", $N43 = "")</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="C43:C44">
     <cfRule type="cellIs" priority="33" operator="equal" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="3">
       <formula>"note"</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="C34:C35">
+  <conditionalFormatting sqref="C43:C44">
     <cfRule type="expression" priority="34" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="4">
-      <formula>AND(AND(NOT($A34 = "end group"), NOT($A34 = "end repeat"), NOT($A34 = "")), $C34 = "")</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="C34:C35">
+      <formula>AND(AND(NOT($A43 = "end group"), NOT($A43 = "end repeat"), NOT($A43 = "")), $C43 = "")</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="C43:C44">
     <cfRule type="expression" priority="35" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="5">
-      <formula>AND($A34="begin repeat", NOT($B34 = ""))</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="C34:C35">
+      <formula>AND($A43="begin repeat", NOT($B43 = ""))</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="C43:C44">
     <cfRule type="expression" priority="36" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="6">
-      <formula>AND($A34="end repeat", $B34 = "", $C34 = "", $D34 = "", $E34 = "", $F34 = "", $G34 = "", $H34 = "", $I34 = "", $J34 = "", $K34 = "", $L34 = "", $M34 = "")</formula>
+      <formula>AND($A43="end repeat", $B43 = "", $C43 = "", $D43 = "", $E43 = "", $F43 = "", $H43 = "", $I43 = "", $J43 = "", $K43 = "", $L43 = "", $M43 = "", $N43 = "")</formula>
     </cfRule>
   </conditionalFormatting>
   <hyperlinks>
@@ -2047,10 +2193,10 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:C19"/>
+  <dimension ref="A1:C25"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="80" zoomScaleNormal="80" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="C4" activeCellId="0" sqref="C4"/>
+      <selection pane="topLeft" activeCell="C22" activeCellId="0" sqref="C22"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -2061,157 +2207,212 @@
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A1" s="9" t="s">
-        <v>149</v>
-      </c>
-      <c r="B1" s="9" t="s">
+      <c r="A1" s="10" t="s">
+        <v>163</v>
+      </c>
+      <c r="B1" s="10" t="s">
         <v>1</v>
       </c>
-      <c r="C1" s="9" t="s">
+      <c r="C1" s="10" t="s">
         <v>2</v>
       </c>
     </row>
     <row r="2" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A2" s="10" t="s">
-        <v>150</v>
+      <c r="A2" s="11" t="s">
+        <v>164</v>
       </c>
       <c r="B2" s="0" t="s">
-        <v>85</v>
-      </c>
-      <c r="C2" s="10" t="s">
-        <v>151</v>
+        <v>105</v>
+      </c>
+      <c r="C2" s="11" t="s">
+        <v>165</v>
       </c>
     </row>
     <row r="3" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A3" s="10" t="s">
-        <v>150</v>
+      <c r="A3" s="11" t="s">
+        <v>164</v>
       </c>
       <c r="B3" s="0" t="s">
-        <v>152</v>
-      </c>
-      <c r="C3" s="10" t="s">
-        <v>153</v>
+        <v>166</v>
+      </c>
+      <c r="C3" s="11" t="s">
+        <v>167</v>
       </c>
     </row>
     <row r="5" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A5" s="0" t="s">
-        <v>154</v>
+        <v>168</v>
       </c>
       <c r="B5" s="0" t="s">
-        <v>155</v>
+        <v>169</v>
       </c>
       <c r="C5" s="0" t="s">
-        <v>156</v>
+        <v>170</v>
       </c>
     </row>
     <row r="6" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A6" s="0" t="s">
-        <v>154</v>
+        <v>168</v>
       </c>
       <c r="B6" s="0" t="s">
-        <v>157</v>
+        <v>171</v>
       </c>
       <c r="C6" s="0" t="s">
-        <v>158</v>
+        <v>172</v>
       </c>
     </row>
     <row r="7" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A7" s="0" t="s">
-        <v>154</v>
+        <v>168</v>
       </c>
       <c r="B7" s="0" t="s">
-        <v>159</v>
+        <v>173</v>
       </c>
       <c r="C7" s="0" t="s">
-        <v>160</v>
+        <v>174</v>
       </c>
     </row>
     <row r="9" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A9" s="0" t="s">
-        <v>161</v>
+        <v>175</v>
       </c>
       <c r="B9" s="0" t="s">
-        <v>162</v>
+        <v>176</v>
       </c>
       <c r="C9" s="0" t="s">
-        <v>163</v>
+        <v>177</v>
       </c>
     </row>
     <row r="10" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A10" s="0" t="s">
-        <v>161</v>
+        <v>175</v>
       </c>
       <c r="B10" s="0" t="s">
-        <v>164</v>
+        <v>178</v>
       </c>
       <c r="C10" s="0" t="s">
-        <v>165</v>
+        <v>179</v>
       </c>
     </row>
     <row r="12" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A12" s="0" t="s">
-        <v>68</v>
+        <v>88</v>
       </c>
       <c r="B12" s="0" t="s">
-        <v>166</v>
+        <v>180</v>
       </c>
       <c r="C12" s="0" t="s">
-        <v>167</v>
+        <v>181</v>
       </c>
     </row>
     <row r="13" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A13" s="0" t="s">
-        <v>68</v>
+        <v>88</v>
       </c>
       <c r="B13" s="0" t="s">
-        <v>168</v>
+        <v>182</v>
       </c>
       <c r="C13" s="0" t="s">
-        <v>169</v>
+        <v>183</v>
       </c>
     </row>
     <row r="15" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A15" s="0" t="s">
-        <v>74</v>
+        <v>94</v>
       </c>
       <c r="B15" s="0" t="s">
-        <v>170</v>
+        <v>184</v>
       </c>
       <c r="C15" s="0" t="s">
-        <v>171</v>
+        <v>185</v>
       </c>
     </row>
     <row r="16" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A16" s="0" t="s">
-        <v>74</v>
+        <v>94</v>
       </c>
       <c r="B16" s="0" t="s">
-        <v>172</v>
+        <v>186</v>
       </c>
       <c r="C16" s="0" t="s">
-        <v>173</v>
+        <v>187</v>
       </c>
     </row>
     <row r="18" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A18" s="0" t="s">
-        <v>48</v>
+        <v>68</v>
       </c>
       <c r="B18" s="0" t="s">
-        <v>174</v>
+        <v>188</v>
       </c>
       <c r="C18" s="0" t="s">
-        <v>175</v>
+        <v>189</v>
       </c>
     </row>
     <row r="19" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A19" s="0" t="s">
-        <v>48</v>
+        <v>68</v>
       </c>
       <c r="B19" s="0" t="s">
-        <v>176</v>
+        <v>190</v>
       </c>
       <c r="C19" s="0" t="s">
-        <v>177</v>
+        <v>191</v>
+      </c>
+    </row>
+    <row r="21" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A21" s="0" t="s">
+        <v>192</v>
+      </c>
+      <c r="B21" s="0" t="s">
+        <v>193</v>
+      </c>
+      <c r="C21" s="0" t="s">
+        <v>194</v>
+      </c>
+    </row>
+    <row r="22" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A22" s="0" t="s">
+        <v>192</v>
+      </c>
+      <c r="B22" s="0" t="s">
+        <v>195</v>
+      </c>
+      <c r="C22" s="0" t="s">
+        <v>196</v>
+      </c>
+    </row>
+    <row r="23" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A23" s="0" t="s">
+        <v>192</v>
+      </c>
+      <c r="B23" s="0" t="s">
+        <v>197</v>
+      </c>
+      <c r="C23" s="0" t="s">
+        <v>198</v>
+      </c>
+    </row>
+    <row r="24" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A24" s="0" t="s">
+        <v>192</v>
+      </c>
+      <c r="B24" s="0" t="s">
+        <v>199</v>
+      </c>
+      <c r="C24" s="0" t="s">
+        <v>200</v>
+      </c>
+    </row>
+    <row r="25" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A25" s="0" t="s">
+        <v>192</v>
+      </c>
+      <c r="B25" s="0" t="s">
+        <v>201</v>
+      </c>
+      <c r="C25" s="0" t="s">
+        <v>202</v>
       </c>
     </row>
   </sheetData>
@@ -2233,7 +2434,7 @@
   <dimension ref="A1:F3"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="80" zoomScaleNormal="80" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="A2" activeCellId="0" sqref="A2"/>
+      <selection pane="topLeft" activeCell="A3" activeCellId="0" sqref="A3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -2246,41 +2447,41 @@
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="28.1" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A1" s="9" t="s">
-        <v>178</v>
-      </c>
-      <c r="B1" s="9" t="s">
-        <v>179</v>
-      </c>
-      <c r="C1" s="9" t="s">
-        <v>180</v>
-      </c>
-      <c r="D1" s="9" t="s">
-        <v>181</v>
-      </c>
-      <c r="E1" s="9" t="s">
-        <v>182</v>
-      </c>
-      <c r="F1" s="9" t="s">
-        <v>183</v>
+      <c r="A1" s="10" t="s">
+        <v>203</v>
+      </c>
+      <c r="B1" s="10" t="s">
+        <v>204</v>
+      </c>
+      <c r="C1" s="10" t="s">
+        <v>205</v>
+      </c>
+      <c r="D1" s="10" t="s">
+        <v>206</v>
+      </c>
+      <c r="E1" s="10" t="s">
+        <v>207</v>
+      </c>
+      <c r="F1" s="10" t="s">
+        <v>208</v>
       </c>
     </row>
     <row r="2" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A2" s="10" t="s">
-        <v>184</v>
-      </c>
-      <c r="B2" s="10" t="s">
-        <v>185</v>
-      </c>
-      <c r="C2" s="11" t="n">
+      <c r="A2" s="11" t="s">
+        <v>209</v>
+      </c>
+      <c r="B2" s="11" t="s">
+        <v>210</v>
+      </c>
+      <c r="C2" s="12" t="n">
         <f aca="true">NOW()</f>
-        <v>43963.662004899</v>
-      </c>
-      <c r="D2" s="10" t="s">
-        <v>186</v>
-      </c>
-      <c r="E2" s="10" t="s">
-        <v>187</v>
+        <v>44032.8427652885</v>
+      </c>
+      <c r="D2" s="11" t="s">
+        <v>211</v>
+      </c>
+      <c r="E2" s="11" t="s">
+        <v>212</v>
       </c>
     </row>
     <row r="3" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>

</xml_diff>